<commit_message>
add manual reload file function for file changes
</commit_message>
<xml_diff>
--- a/pharma-sample-data.xlsx
+++ b/pharma-sample-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Item Code</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>Allergy Eye Drops</t>
+  </si>
+  <si>
+    <t>Neozep</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -238,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -266,6 +272,15 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -578,15 +593,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="10.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
@@ -1147,10 +1162,10 @@
         <v>52</v>
       </c>
       <c r="C51" s="9">
-        <v>5.99</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -1160,6 +1175,24 @@
       <c r="C52" s="6">
         <v>7.49</v>
       </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18">
+      <c r="A53" s="10">
+        <v>52</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="11">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+      <c r="A54" s="4"/>
+      <c r="B54" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add reload function to support file changes while server running
</commit_message>
<xml_diff>
--- a/pharma-sample-data.xlsx
+++ b/pharma-sample-data.xlsx
@@ -1162,7 +1162,7 @@
         <v>52</v>
       </c>
       <c r="C51" s="9">
-        <v>5</v>
+        <v>5.09</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18">
@@ -1184,7 +1184,7 @@
         <v>54</v>
       </c>
       <c r="C53" s="11">
-        <v>1.09</v>
+        <v>5.09</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">

</xml_diff>